<commit_message>
continua graduação + planejamento
</commit_message>
<xml_diff>
--- a/dados_graduacao/Tabela12_DEG-2019.xlsx
+++ b/dados_graduacao/Tabela12_DEG-2019.xlsx
@@ -1162,8 +1162,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1203,6 +1201,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1615,53 +1615,53 @@
     </row>
     <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="34"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="28"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="35" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="36"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:15" s="1" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1670,17 +1670,17 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1713,17 +1713,17 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
@@ -1842,17 +1842,17 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
@@ -2029,17 +2029,17 @@
       </c>
     </row>
     <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10">
@@ -2100,17 +2100,17 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
     </row>
     <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
@@ -2200,17 +2200,17 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="25"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10">
@@ -2387,17 +2387,17 @@
       </c>
     </row>
     <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
     </row>
     <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10">
@@ -2487,17 +2487,17 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
@@ -2558,17 +2558,17 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="25" t="s">
+      <c r="A41" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="23"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
     </row>
     <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10">
@@ -2658,17 +2658,17 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="25" t="s">
+      <c r="A45" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10">
@@ -2758,17 +2758,17 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10">
@@ -2945,17 +2945,17 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="25"/>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23"/>
+      <c r="I56" s="23"/>
     </row>
     <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10">
@@ -2987,17 +2987,17 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="25" t="s">
+      <c r="A58" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
     </row>
     <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10">
@@ -3174,17 +3174,17 @@
       </c>
     </row>
     <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="25" t="s">
+      <c r="A65" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
-      <c r="D65" s="25"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="25"/>
-      <c r="I65" s="25"/>
+      <c r="B65" s="23"/>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="23"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
     </row>
     <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10">
@@ -3419,17 +3419,17 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="25" t="s">
+      <c r="A74" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
-      <c r="G74" s="25"/>
-      <c r="H74" s="25"/>
-      <c r="I74" s="25"/>
+      <c r="B74" s="23"/>
+      <c r="C74" s="23"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
+      <c r="I74" s="23"/>
     </row>
     <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10">
@@ -3577,17 +3577,17 @@
       </c>
     </row>
     <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="25" t="s">
+      <c r="A80" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="25"/>
-      <c r="F80" s="25"/>
-      <c r="G80" s="25"/>
-      <c r="H80" s="25"/>
-      <c r="I80" s="25"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="23"/>
+      <c r="H80" s="23"/>
+      <c r="I80" s="23"/>
     </row>
     <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="10">
@@ -3735,17 +3735,17 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="25" t="s">
+      <c r="A86" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="25"/>
-      <c r="C86" s="25"/>
-      <c r="D86" s="25"/>
-      <c r="E86" s="25"/>
-      <c r="F86" s="25"/>
-      <c r="G86" s="25"/>
-      <c r="H86" s="25"/>
-      <c r="I86" s="25"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23"/>
+      <c r="D86" s="23"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
+      <c r="I86" s="23"/>
     </row>
     <row r="87" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="10">
@@ -3864,17 +3864,17 @@
       </c>
     </row>
     <row r="91" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="25" t="s">
+      <c r="A91" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="25"/>
-      <c r="C91" s="25"/>
-      <c r="D91" s="25"/>
-      <c r="E91" s="25"/>
-      <c r="F91" s="25"/>
-      <c r="G91" s="25"/>
-      <c r="H91" s="25"/>
-      <c r="I91" s="25"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
+      <c r="I91" s="23"/>
     </row>
     <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92" s="10">
@@ -4370,17 +4370,17 @@
       </c>
     </row>
     <row r="109" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="25" t="s">
+      <c r="A109" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B109" s="25"/>
-      <c r="C109" s="25"/>
-      <c r="D109" s="25"/>
-      <c r="E109" s="25"/>
-      <c r="F109" s="25"/>
-      <c r="G109" s="25"/>
-      <c r="H109" s="25"/>
-      <c r="I109" s="25"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="23"/>
+      <c r="I109" s="23"/>
     </row>
     <row r="110" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A110" s="10">
@@ -4586,17 +4586,17 @@
       </c>
     </row>
     <row r="117" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="25" t="s">
+      <c r="A117" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="B117" s="25"/>
-      <c r="C117" s="25"/>
-      <c r="D117" s="25"/>
-      <c r="E117" s="25"/>
-      <c r="F117" s="25"/>
-      <c r="G117" s="25"/>
-      <c r="H117" s="25"/>
-      <c r="I117" s="25"/>
+      <c r="B117" s="23"/>
+      <c r="C117" s="23"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="23"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="23"/>
+      <c r="I117" s="23"/>
     </row>
     <row r="118" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="10">
@@ -4686,17 +4686,17 @@
       </c>
     </row>
     <row r="121" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="25" t="s">
+      <c r="A121" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="B121" s="25"/>
-      <c r="C121" s="25"/>
-      <c r="D121" s="25"/>
-      <c r="E121" s="25"/>
-      <c r="F121" s="25"/>
-      <c r="G121" s="25"/>
-      <c r="H121" s="25"/>
-      <c r="I121" s="25"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="23"/>
+      <c r="H121" s="23"/>
+      <c r="I121" s="23"/>
     </row>
     <row r="122" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="10">
@@ -4786,17 +4786,17 @@
       </c>
     </row>
     <row r="125" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="25" t="s">
+      <c r="A125" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="B125" s="25"/>
-      <c r="C125" s="25"/>
-      <c r="D125" s="25"/>
-      <c r="E125" s="25"/>
-      <c r="F125" s="25"/>
-      <c r="G125" s="25"/>
-      <c r="H125" s="25"/>
-      <c r="I125" s="25"/>
+      <c r="B125" s="23"/>
+      <c r="C125" s="23"/>
+      <c r="D125" s="23"/>
+      <c r="E125" s="23"/>
+      <c r="F125" s="23"/>
+      <c r="G125" s="23"/>
+      <c r="H125" s="23"/>
+      <c r="I125" s="23"/>
     </row>
     <row r="126" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="10">
@@ -5118,17 +5118,17 @@
       </c>
     </row>
     <row r="137" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="25" t="s">
+      <c r="A137" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="B137" s="25"/>
-      <c r="C137" s="25"/>
-      <c r="D137" s="25"/>
-      <c r="E137" s="25"/>
-      <c r="F137" s="25"/>
-      <c r="G137" s="25"/>
-      <c r="H137" s="25"/>
-      <c r="I137" s="25"/>
+      <c r="B137" s="23"/>
+      <c r="C137" s="23"/>
+      <c r="D137" s="23"/>
+      <c r="E137" s="23"/>
+      <c r="F137" s="23"/>
+      <c r="G137" s="23"/>
+      <c r="H137" s="23"/>
+      <c r="I137" s="23"/>
     </row>
     <row r="138" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="10">
@@ -5595,17 +5595,17 @@
       </c>
     </row>
     <row r="154" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A154" s="25" t="s">
+      <c r="A154" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="B154" s="25"/>
-      <c r="C154" s="25"/>
-      <c r="D154" s="25"/>
-      <c r="E154" s="25"/>
-      <c r="F154" s="25"/>
-      <c r="G154" s="25"/>
-      <c r="H154" s="25"/>
-      <c r="I154" s="25"/>
+      <c r="B154" s="23"/>
+      <c r="C154" s="23"/>
+      <c r="D154" s="23"/>
+      <c r="E154" s="23"/>
+      <c r="F154" s="23"/>
+      <c r="G154" s="23"/>
+      <c r="H154" s="23"/>
+      <c r="I154" s="23"/>
     </row>
     <row r="155" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A155" s="10">
@@ -5695,17 +5695,17 @@
       </c>
     </row>
     <row r="158" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A158" s="25" t="s">
+      <c r="A158" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="B158" s="25"/>
-      <c r="C158" s="25"/>
-      <c r="D158" s="25"/>
-      <c r="E158" s="25"/>
-      <c r="F158" s="25"/>
-      <c r="G158" s="25"/>
-      <c r="H158" s="25"/>
-      <c r="I158" s="25"/>
+      <c r="B158" s="23"/>
+      <c r="C158" s="23"/>
+      <c r="D158" s="23"/>
+      <c r="E158" s="23"/>
+      <c r="F158" s="23"/>
+      <c r="G158" s="23"/>
+      <c r="H158" s="23"/>
+      <c r="I158" s="23"/>
     </row>
     <row r="159" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A159" s="10">
@@ -5737,17 +5737,17 @@
       </c>
     </row>
     <row r="160" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A160" s="25" t="s">
+      <c r="A160" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="B160" s="25"/>
-      <c r="C160" s="25"/>
-      <c r="D160" s="25"/>
-      <c r="E160" s="25"/>
-      <c r="F160" s="25"/>
-      <c r="G160" s="25"/>
-      <c r="H160" s="25"/>
-      <c r="I160" s="25"/>
+      <c r="B160" s="23"/>
+      <c r="C160" s="23"/>
+      <c r="D160" s="23"/>
+      <c r="E160" s="23"/>
+      <c r="F160" s="23"/>
+      <c r="G160" s="23"/>
+      <c r="H160" s="23"/>
+      <c r="I160" s="23"/>
     </row>
     <row r="161" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A161" s="10">
@@ -5866,17 +5866,17 @@
       </c>
     </row>
     <row r="165" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A165" s="25" t="s">
+      <c r="A165" s="23" t="s">
         <v>165</v>
       </c>
-      <c r="B165" s="25"/>
-      <c r="C165" s="25"/>
-      <c r="D165" s="25"/>
-      <c r="E165" s="25"/>
-      <c r="F165" s="25"/>
-      <c r="G165" s="25"/>
-      <c r="H165" s="25"/>
-      <c r="I165" s="25"/>
+      <c r="B165" s="23"/>
+      <c r="C165" s="23"/>
+      <c r="D165" s="23"/>
+      <c r="E165" s="23"/>
+      <c r="F165" s="23"/>
+      <c r="G165" s="23"/>
+      <c r="H165" s="23"/>
+      <c r="I165" s="23"/>
     </row>
     <row r="166" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A166" s="10">
@@ -5908,33 +5908,57 @@
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A167" s="23"/>
-      <c r="B167" s="23"/>
+      <c r="A167" s="36"/>
+      <c r="B167" s="36"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A168" s="24" t="s">
+      <c r="A168" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="B168" s="24"/>
+      <c r="B168" s="37"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A169" s="24" t="s">
+      <c r="A169" s="37" t="s">
         <v>265</v>
       </c>
-      <c r="B169" s="24"/>
-      <c r="C169" s="24"/>
-      <c r="D169" s="24"/>
-      <c r="E169" s="24"/>
-      <c r="F169" s="24"/>
-      <c r="G169" s="24"/>
-      <c r="H169" s="24"/>
-      <c r="I169" s="24"/>
+      <c r="B169" s="37"/>
+      <c r="C169" s="37"/>
+      <c r="D169" s="37"/>
+      <c r="E169" s="37"/>
+      <c r="F169" s="37"/>
+      <c r="G169" s="37"/>
+      <c r="H169" s="37"/>
+      <c r="I169" s="37"/>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G174" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="A169:I169"/>
+    <mergeCell ref="A125:I125"/>
+    <mergeCell ref="A137:I137"/>
+    <mergeCell ref="A154:I154"/>
+    <mergeCell ref="A158:I158"/>
+    <mergeCell ref="A160:I160"/>
+    <mergeCell ref="A165:I165"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A121:I121"/>
+    <mergeCell ref="A45:I45"/>
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A56:I56"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="A74:I74"/>
+    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="A91:I91"/>
+    <mergeCell ref="A109:I109"/>
+    <mergeCell ref="A117:I117"/>
+    <mergeCell ref="A41:I41"/>
     <mergeCell ref="A20:I20"/>
     <mergeCell ref="A23:I23"/>
     <mergeCell ref="A27:I27"/>
@@ -5950,30 +5974,6 @@
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A38:I38"/>
-    <mergeCell ref="A121:I121"/>
-    <mergeCell ref="A45:I45"/>
-    <mergeCell ref="A49:I49"/>
-    <mergeCell ref="A56:I56"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="A74:I74"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="A91:I91"/>
-    <mergeCell ref="A109:I109"/>
-    <mergeCell ref="A117:I117"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A167:B167"/>
-    <mergeCell ref="A168:B168"/>
-    <mergeCell ref="A169:I169"/>
-    <mergeCell ref="A125:I125"/>
-    <mergeCell ref="A137:I137"/>
-    <mergeCell ref="A154:I154"/>
-    <mergeCell ref="A158:I158"/>
-    <mergeCell ref="A160:I160"/>
-    <mergeCell ref="A165:I165"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -5983,9 +5983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O167"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10245,5 +10243,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>